<commit_message>
fixed a few errors in new data
</commit_message>
<xml_diff>
--- a/data/Species DB.xlsx
+++ b/data/Species DB.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox (Personal)\Webpages\TaxonomyMonographBuilder\fiddlercrab.info\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="8130" yWindow="525" windowWidth="10500" windowHeight="13155" activeTab="5"/>
   </bookViews>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10365" uniqueCount="3285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10365" uniqueCount="3286">
   <si>
     <t>acuta</t>
   </si>
@@ -9882,12 +9877,15 @@
   </si>
   <si>
     <t>pugilator;pugillator;pugilatus;pigilator;puqilato;pugilato</t>
+  </si>
+  <si>
+    <t>flammula;flamula</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -10067,7 +10065,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10100,26 +10098,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10152,23 +10133,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -10354,13 +10318,13 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="21.25" customWidth="1"/>
+    <col min="6" max="6" width="9.625" customWidth="1"/>
+    <col min="7" max="7" width="19.125" customWidth="1"/>
     <col min="8" max="8" width="77" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.125" customWidth="1"/>
+    <col min="11" max="11" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
@@ -15178,9 +15142,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="2" max="2" width="27.375" customWidth="1"/>
+    <col min="3" max="3" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -15459,7 +15423,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="5.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -22457,9 +22421,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="43.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.75" customWidth="1"/>
+    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="8" max="8" width="43.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
@@ -25196,17 +25160,17 @@
       <selection activeCell="I614" sqref="I614"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="15"/>
-    <col min="3" max="3" width="18.42578125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="15" customWidth="1"/>
+    <col min="1" max="2" width="9.125" style="15"/>
+    <col min="3" max="3" width="18.375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="6.75" style="15" customWidth="1"/>
     <col min="5" max="6" width="21" style="15" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="15" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="15" customWidth="1"/>
-    <col min="9" max="16" width="9.140625" style="15"/>
-    <col min="17" max="17" width="9.5703125" style="15" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="15"/>
+    <col min="7" max="7" width="6.75" style="15" customWidth="1"/>
+    <col min="8" max="8" width="9.375" style="15" customWidth="1"/>
+    <col min="9" max="16" width="9.125" style="15"/>
+    <col min="17" max="17" width="9.625" style="15" customWidth="1"/>
+    <col min="18" max="16384" width="9.125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -44217,19 +44181,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B59" sqref="A1:G201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="38.625" customWidth="1"/>
+    <col min="3" max="3" width="9.75" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="18.875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -45571,7 +45535,7 @@
         <v>26</v>
       </c>
       <c r="B59" t="s">
-        <v>26</v>
+        <v>3285</v>
       </c>
       <c r="C59" t="s">
         <v>26</v>
@@ -48874,11 +48838,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.625" customWidth="1"/>
+    <col min="2" max="2" width="13.875" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -50289,7 +50253,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.375" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
typo in common name text
</commit_message>
<xml_diff>
--- a/data/Species DB.xlsx
+++ b/data/Species DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8130" yWindow="525" windowWidth="10500" windowHeight="13155" activeTab="2"/>
+    <workbookView xWindow="8130" yWindow="525" windowWidth="10500" windowHeight="13155" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="species_info" sheetId="1" r:id="rId1"/>
@@ -9681,9 +9681,6 @@
     <t>Southern Calling Fiddler Crab; Two-toned Fiddler Crab</t>
   </si>
   <si>
-    <t>Less commonly used in English, the term &amp;ldquo;Calling Crab&amp;rdquo; derives from one of the earliest scientific papers to include these crabs, [[Rumphius1705,.out]]. Rumphius names one of his species &lt;em class="species"&gt;Cancer vocans&lt;/em&gt;  which is Latin for &amp;ldquo;calling crab&amp;rdquo; or &amp;ldquo;gesturing crab.&amp;rdquo; He also reports the name &amp;ldquo;Cattam Pangel&amp;rdquo; which appears to most likely be a form of Malay meaning &amp;ldquo;summoning crab,&amp;rdquo; and is probably from where he derived the Latin name. In a later work [[Rumphius1711,.in]] he includes a Dutch name &amp;ldquo;Roepende Krabbe,&amp;rdquo; which also translates to Calling Crab.</t>
-  </si>
-  <si>
     <t>Blanchard1890</t>
   </si>
   <si>
@@ -9904,6 +9901,9 @@
   </si>
   <si>
     <t>Sanya, China. Photo provided by Jeff Zhang.</t>
+  </si>
+  <si>
+    <t>Less commonly used in English, the term &amp;ldquo;Calling Crab&amp;rdquo; derives from one of the earliest scientific papers to include these crabs, [[Rumphius1705,.out]]. Rumphius names one of his species &lt;em class="species"&gt;Cancer vocans&lt;/em&gt;  which is Latin for &amp;ldquo;calling crab&amp;rdquo; or &amp;ldquo;gesturing crab.&amp;rdquo; He also reports the name &amp;ldquo;Cattam Pangel&amp;rdquo; which appears to most likely be a form of Malay meaning &amp;ldquo;summoning crab,&amp;rdquo; and is probably from where he derived the Latin name. In a later work ([[Rumphius1711,.in]]) he includes a Dutch name &amp;ldquo;Roepende Krabbe,&amp;rdquo; which also translates to Calling Crab.</t>
   </si>
 </sst>
 </file>
@@ -11248,7 +11248,7 @@
         <v>423</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>3264</v>
+        <v>3263</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>509</v>
@@ -14328,7 +14328,7 @@
         <v>206</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>3263</v>
+        <v>3262</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>731</v>
@@ -14812,7 +14812,7 @@
         <v>232</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>3260</v>
+        <v>3259</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>723</v>
@@ -15441,7 +15441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C662"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A598" workbookViewId="0">
+    <sheetView topLeftCell="A598" workbookViewId="0">
       <selection activeCell="B613" sqref="B613"/>
     </sheetView>
   </sheetViews>
@@ -15557,7 +15557,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -15766,7 +15766,7 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -15777,7 +15777,7 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -15788,7 +15788,7 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -15799,7 +15799,7 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -15810,7 +15810,7 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -15821,7 +15821,7 @@
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -15865,7 +15865,7 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -15876,7 +15876,7 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -15887,7 +15887,7 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -15898,7 +15898,7 @@
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -15909,7 +15909,7 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>3287</v>
+        <v>3286</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -15920,7 +15920,7 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>3286</v>
+        <v>3285</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -16162,7 +16162,7 @@
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>3288</v>
+        <v>3287</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -16261,7 +16261,7 @@
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -16272,7 +16272,7 @@
         <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -16283,7 +16283,7 @@
         <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -16294,7 +16294,7 @@
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -16305,7 +16305,7 @@
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -16316,7 +16316,7 @@
         <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -16327,7 +16327,7 @@
         <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -16338,7 +16338,7 @@
         <v>10</v>
       </c>
       <c r="C81" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -16349,7 +16349,7 @@
         <v>11</v>
       </c>
       <c r="C82" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -16360,7 +16360,7 @@
         <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -16371,7 +16371,7 @@
         <v>13</v>
       </c>
       <c r="C84" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -16382,7 +16382,7 @@
         <v>14</v>
       </c>
       <c r="C85" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -16393,7 +16393,7 @@
         <v>15</v>
       </c>
       <c r="C86" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -16404,7 +16404,7 @@
         <v>16</v>
       </c>
       <c r="C87" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -16415,7 +16415,7 @@
         <v>17</v>
       </c>
       <c r="C88" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -16426,7 +16426,7 @@
         <v>18</v>
       </c>
       <c r="C89" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -16437,7 +16437,7 @@
         <v>19</v>
       </c>
       <c r="C90" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -16448,7 +16448,7 @@
         <v>20</v>
       </c>
       <c r="C91" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -16459,7 +16459,7 @@
         <v>21</v>
       </c>
       <c r="C92" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -16470,7 +16470,7 @@
         <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -16481,7 +16481,7 @@
         <v>23</v>
       </c>
       <c r="C94" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -16492,7 +16492,7 @@
         <v>24</v>
       </c>
       <c r="C95" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -16503,7 +16503,7 @@
         <v>25</v>
       </c>
       <c r="C96" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -16514,7 +16514,7 @@
         <v>26</v>
       </c>
       <c r="C97" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -16591,7 +16591,7 @@
         <v>7</v>
       </c>
       <c r="C104" t="s">
-        <v>3287</v>
+        <v>3286</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -16657,7 +16657,7 @@
         <v>6</v>
       </c>
       <c r="C110" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -16668,7 +16668,7 @@
         <v>7</v>
       </c>
       <c r="C111" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -16679,7 +16679,7 @@
         <v>8</v>
       </c>
       <c r="C112" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -16690,7 +16690,7 @@
         <v>9</v>
       </c>
       <c r="C113" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -16701,7 +16701,7 @@
         <v>10</v>
       </c>
       <c r="C114" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -16712,7 +16712,7 @@
         <v>11</v>
       </c>
       <c r="C115" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -16723,7 +16723,7 @@
         <v>12</v>
       </c>
       <c r="C116" t="s">
-        <v>3289</v>
+        <v>3288</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -17295,7 +17295,7 @@
         <v>2</v>
       </c>
       <c r="C168" t="s">
-        <v>3290</v>
+        <v>3289</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -17493,7 +17493,7 @@
         <v>12</v>
       </c>
       <c r="C186" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -17504,7 +17504,7 @@
         <v>13</v>
       </c>
       <c r="C187" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -17515,7 +17515,7 @@
         <v>14</v>
       </c>
       <c r="C188" t="s">
-        <v>3289</v>
+        <v>3288</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -17614,7 +17614,7 @@
         <v>2</v>
       </c>
       <c r="C197" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -17625,7 +17625,7 @@
         <v>3</v>
       </c>
       <c r="C198" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -17636,7 +17636,7 @@
         <v>4</v>
       </c>
       <c r="C199" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -17647,7 +17647,7 @@
         <v>5</v>
       </c>
       <c r="C200" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -17658,7 +17658,7 @@
         <v>6</v>
       </c>
       <c r="C201" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -17669,7 +17669,7 @@
         <v>7</v>
       </c>
       <c r="C202" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -17680,7 +17680,7 @@
         <v>8</v>
       </c>
       <c r="C203" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -17691,7 +17691,7 @@
         <v>9</v>
       </c>
       <c r="C204" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -17702,7 +17702,7 @@
         <v>10</v>
       </c>
       <c r="C205" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -17713,7 +17713,7 @@
         <v>11</v>
       </c>
       <c r="C206" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -17724,7 +17724,7 @@
         <v>12</v>
       </c>
       <c r="C207" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -17889,7 +17889,7 @@
         <v>5</v>
       </c>
       <c r="C222" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -17900,7 +17900,7 @@
         <v>6</v>
       </c>
       <c r="C223" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -17911,7 +17911,7 @@
         <v>7</v>
       </c>
       <c r="C224" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -17922,7 +17922,7 @@
         <v>8</v>
       </c>
       <c r="C225" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -17933,7 +17933,7 @@
         <v>9</v>
       </c>
       <c r="C226" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -17944,7 +17944,7 @@
         <v>10</v>
       </c>
       <c r="C227" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -17955,7 +17955,7 @@
         <v>11</v>
       </c>
       <c r="C228" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -17966,7 +17966,7 @@
         <v>12</v>
       </c>
       <c r="C229" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -17977,7 +17977,7 @@
         <v>13</v>
       </c>
       <c r="C230" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -17988,7 +17988,7 @@
         <v>14</v>
       </c>
       <c r="C231" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -17999,7 +17999,7 @@
         <v>15</v>
       </c>
       <c r="C232" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -18010,7 +18010,7 @@
         <v>16</v>
       </c>
       <c r="C233" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -18021,7 +18021,7 @@
         <v>17</v>
       </c>
       <c r="C234" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -18032,7 +18032,7 @@
         <v>18</v>
       </c>
       <c r="C235" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -18043,7 +18043,7 @@
         <v>19</v>
       </c>
       <c r="C236" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -18087,7 +18087,7 @@
         <v>4</v>
       </c>
       <c r="C240" t="s">
-        <v>3243</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -18098,7 +18098,7 @@
         <v>5</v>
       </c>
       <c r="C241" t="s">
-        <v>3243</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -18109,7 +18109,7 @@
         <v>6</v>
       </c>
       <c r="C242" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -18120,7 +18120,7 @@
         <v>7</v>
       </c>
       <c r="C243" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -18131,7 +18131,7 @@
         <v>8</v>
       </c>
       <c r="C244" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -18142,18 +18142,18 @@
         <v>9</v>
       </c>
       <c r="C245" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>3245</v>
+        <v>3244</v>
       </c>
       <c r="B246">
         <v>1</v>
       </c>
       <c r="C246" t="s">
-        <v>3246</v>
+        <v>3245</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -18164,7 +18164,7 @@
         <v>10</v>
       </c>
       <c r="C247" t="s">
-        <v>3289</v>
+        <v>3288</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -18494,7 +18494,7 @@
         <v>5</v>
       </c>
       <c r="C277" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -18505,7 +18505,7 @@
         <v>6</v>
       </c>
       <c r="C278" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -18516,7 +18516,7 @@
         <v>7</v>
       </c>
       <c r="C279" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -18527,7 +18527,7 @@
         <v>8</v>
       </c>
       <c r="C280" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -18538,7 +18538,7 @@
         <v>9</v>
       </c>
       <c r="C281" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -18549,7 +18549,7 @@
         <v>10</v>
       </c>
       <c r="C282" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -18560,7 +18560,7 @@
         <v>11</v>
       </c>
       <c r="C283" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -18571,7 +18571,7 @@
         <v>12</v>
       </c>
       <c r="C284" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -18582,7 +18582,7 @@
         <v>13</v>
       </c>
       <c r="C285" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -18593,7 +18593,7 @@
         <v>14</v>
       </c>
       <c r="C286" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -18615,7 +18615,7 @@
         <v>2</v>
       </c>
       <c r="C288" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -18648,7 +18648,7 @@
         <v>3</v>
       </c>
       <c r="C291" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -18659,7 +18659,7 @@
         <v>4</v>
       </c>
       <c r="C292" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -18670,7 +18670,7 @@
         <v>5</v>
       </c>
       <c r="C293" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -18681,7 +18681,7 @@
         <v>6</v>
       </c>
       <c r="C294" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -18692,7 +18692,7 @@
         <v>1</v>
       </c>
       <c r="C295" t="s">
-        <v>3291</v>
+        <v>3290</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -19176,7 +19176,7 @@
         <v>1</v>
       </c>
       <c r="C339" t="s">
-        <v>3291</v>
+        <v>3290</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
@@ -19385,7 +19385,7 @@
         <v>9</v>
       </c>
       <c r="C358" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
@@ -19396,7 +19396,7 @@
         <v>10</v>
       </c>
       <c r="C359" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
@@ -19407,7 +19407,7 @@
         <v>11</v>
       </c>
       <c r="C360" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
@@ -19418,7 +19418,7 @@
         <v>12</v>
       </c>
       <c r="C361" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
@@ -19429,7 +19429,7 @@
         <v>13</v>
       </c>
       <c r="C362" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
@@ -19440,7 +19440,7 @@
         <v>14</v>
       </c>
       <c r="C363" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
@@ -19451,7 +19451,7 @@
         <v>15</v>
       </c>
       <c r="C364" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
@@ -19462,7 +19462,7 @@
         <v>16</v>
       </c>
       <c r="C365" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
@@ -19473,7 +19473,7 @@
         <v>17</v>
       </c>
       <c r="C366" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
@@ -19484,7 +19484,7 @@
         <v>18</v>
       </c>
       <c r="C367" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
@@ -19495,7 +19495,7 @@
         <v>19</v>
       </c>
       <c r="C368" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
@@ -19506,7 +19506,7 @@
         <v>20</v>
       </c>
       <c r="C369" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -19517,7 +19517,7 @@
         <v>21</v>
       </c>
       <c r="C370" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
@@ -19528,7 +19528,7 @@
         <v>22</v>
       </c>
       <c r="C371" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
@@ -19539,7 +19539,7 @@
         <v>23</v>
       </c>
       <c r="C372" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
@@ -19550,7 +19550,7 @@
         <v>24</v>
       </c>
       <c r="C373" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
@@ -19561,7 +19561,7 @@
         <v>25</v>
       </c>
       <c r="C374" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
@@ -19572,7 +19572,7 @@
         <v>26</v>
       </c>
       <c r="C375" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
@@ -19583,7 +19583,7 @@
         <v>27</v>
       </c>
       <c r="C376" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
@@ -19594,7 +19594,7 @@
         <v>28</v>
       </c>
       <c r="C377" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
@@ -19605,7 +19605,7 @@
         <v>29</v>
       </c>
       <c r="C378" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
@@ -19616,7 +19616,7 @@
         <v>30</v>
       </c>
       <c r="C379" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
@@ -19627,7 +19627,7 @@
         <v>31</v>
       </c>
       <c r="C380" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
@@ -19638,7 +19638,7 @@
         <v>32</v>
       </c>
       <c r="C381" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
@@ -19671,7 +19671,7 @@
         <v>1</v>
       </c>
       <c r="C384" t="s">
-        <v>3292</v>
+        <v>3291</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
@@ -19792,7 +19792,7 @@
         <v>3</v>
       </c>
       <c r="C395" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
@@ -19803,7 +19803,7 @@
         <v>4</v>
       </c>
       <c r="C396" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
@@ -19814,7 +19814,7 @@
         <v>5</v>
       </c>
       <c r="C397" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
@@ -19825,7 +19825,7 @@
         <v>6</v>
       </c>
       <c r="C398" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
@@ -19836,7 +19836,7 @@
         <v>7</v>
       </c>
       <c r="C399" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
@@ -20034,7 +20034,7 @@
         <v>3</v>
       </c>
       <c r="C417" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
@@ -20045,7 +20045,7 @@
         <v>4</v>
       </c>
       <c r="C418" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
@@ -20056,7 +20056,7 @@
         <v>5</v>
       </c>
       <c r="C419" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
@@ -20067,7 +20067,7 @@
         <v>6</v>
       </c>
       <c r="C420" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
@@ -20078,7 +20078,7 @@
         <v>7</v>
       </c>
       <c r="C421" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
@@ -20089,7 +20089,7 @@
         <v>8</v>
       </c>
       <c r="C422" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
@@ -20100,7 +20100,7 @@
         <v>9</v>
       </c>
       <c r="C423" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
@@ -20342,7 +20342,7 @@
         <v>2</v>
       </c>
       <c r="C445" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.25">
@@ -20353,7 +20353,7 @@
         <v>3</v>
       </c>
       <c r="C446" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.25">
@@ -20364,7 +20364,7 @@
         <v>4</v>
       </c>
       <c r="C447" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.25">
@@ -20375,7 +20375,7 @@
         <v>5</v>
       </c>
       <c r="C448" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.25">
@@ -20386,7 +20386,7 @@
         <v>6</v>
       </c>
       <c r="C449" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.25">
@@ -20397,7 +20397,7 @@
         <v>7</v>
       </c>
       <c r="C450" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.25">
@@ -20408,7 +20408,7 @@
         <v>8</v>
       </c>
       <c r="C451" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.25">
@@ -20419,7 +20419,7 @@
         <v>9</v>
       </c>
       <c r="C452" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.25">
@@ -20430,7 +20430,7 @@
         <v>10</v>
       </c>
       <c r="C453" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.25">
@@ -20441,7 +20441,7 @@
         <v>11</v>
       </c>
       <c r="C454" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.25">
@@ -20452,7 +20452,7 @@
         <v>12</v>
       </c>
       <c r="C455" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.25">
@@ -20496,7 +20496,7 @@
         <v>4</v>
       </c>
       <c r="C459" t="s">
-        <v>3291</v>
+        <v>3290</v>
       </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.25">
@@ -20782,7 +20782,7 @@
         <v>1</v>
       </c>
       <c r="C485" t="s">
-        <v>3289</v>
+        <v>3288</v>
       </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.25">
@@ -20815,7 +20815,7 @@
         <v>3</v>
       </c>
       <c r="C488" t="s">
-        <v>3289</v>
+        <v>3288</v>
       </c>
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.25">
@@ -20859,7 +20859,7 @@
         <v>4</v>
       </c>
       <c r="C492" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.25">
@@ -20870,7 +20870,7 @@
         <v>5</v>
       </c>
       <c r="C493" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.25">
@@ -20881,7 +20881,7 @@
         <v>6</v>
       </c>
       <c r="C494" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.25">
@@ -20892,7 +20892,7 @@
         <v>7</v>
       </c>
       <c r="C495" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.25">
@@ -20903,7 +20903,7 @@
         <v>8</v>
       </c>
       <c r="C496" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.25">
@@ -20914,7 +20914,7 @@
         <v>9</v>
       </c>
       <c r="C497" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.25">
@@ -20925,7 +20925,7 @@
         <v>10</v>
       </c>
       <c r="C498" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.25">
@@ -20958,7 +20958,7 @@
         <v>3</v>
       </c>
       <c r="C501" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.25">
@@ -20969,7 +20969,7 @@
         <v>4</v>
       </c>
       <c r="C502" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.25">
@@ -20980,7 +20980,7 @@
         <v>5</v>
       </c>
       <c r="C503" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.25">
@@ -20991,7 +20991,7 @@
         <v>6</v>
       </c>
       <c r="C504" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.25">
@@ -21002,7 +21002,7 @@
         <v>7</v>
       </c>
       <c r="C505" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.25">
@@ -21024,7 +21024,7 @@
         <v>2</v>
       </c>
       <c r="C507" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.25">
@@ -21035,7 +21035,7 @@
         <v>3</v>
       </c>
       <c r="C508" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.25">
@@ -21046,7 +21046,7 @@
         <v>4</v>
       </c>
       <c r="C509" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.25">
@@ -21057,7 +21057,7 @@
         <v>5</v>
       </c>
       <c r="C510" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="511" spans="1:3" x14ac:dyDescent="0.25">
@@ -21068,7 +21068,7 @@
         <v>6</v>
       </c>
       <c r="C511" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.25">
@@ -21079,7 +21079,7 @@
         <v>7</v>
       </c>
       <c r="C512" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.25">
@@ -21090,7 +21090,7 @@
         <v>8</v>
       </c>
       <c r="C513" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.25">
@@ -21101,7 +21101,7 @@
         <v>9</v>
       </c>
       <c r="C514" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="515" spans="1:3" x14ac:dyDescent="0.25">
@@ -21112,7 +21112,7 @@
         <v>1</v>
       </c>
       <c r="C515" t="s">
-        <v>3286</v>
+        <v>3285</v>
       </c>
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.25">
@@ -21332,7 +21332,7 @@
         <v>6</v>
       </c>
       <c r="C535" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="536" spans="1:3" x14ac:dyDescent="0.25">
@@ -21343,7 +21343,7 @@
         <v>7</v>
       </c>
       <c r="C536" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.25">
@@ -21354,7 +21354,7 @@
         <v>8</v>
       </c>
       <c r="C537" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="538" spans="1:3" x14ac:dyDescent="0.25">
@@ -21365,7 +21365,7 @@
         <v>9</v>
       </c>
       <c r="C538" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.25">
@@ -21376,7 +21376,7 @@
         <v>10</v>
       </c>
       <c r="C539" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.25">
@@ -21387,7 +21387,7 @@
         <v>11</v>
       </c>
       <c r="C540" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.25">
@@ -21398,7 +21398,7 @@
         <v>12</v>
       </c>
       <c r="C541" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.25">
@@ -21409,7 +21409,7 @@
         <v>13</v>
       </c>
       <c r="C542" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="543" spans="1:3" x14ac:dyDescent="0.25">
@@ -21453,7 +21453,7 @@
         <v>4</v>
       </c>
       <c r="C546" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="547" spans="1:3" x14ac:dyDescent="0.25">
@@ -21464,7 +21464,7 @@
         <v>5</v>
       </c>
       <c r="C547" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="548" spans="1:3" x14ac:dyDescent="0.25">
@@ -21475,7 +21475,7 @@
         <v>6</v>
       </c>
       <c r="C548" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.25">
@@ -21728,7 +21728,7 @@
         <v>4</v>
       </c>
       <c r="C571" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="572" spans="1:3" x14ac:dyDescent="0.25">
@@ -21739,7 +21739,7 @@
         <v>5</v>
       </c>
       <c r="C572" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="573" spans="1:3" x14ac:dyDescent="0.25">
@@ -21750,7 +21750,7 @@
         <v>6</v>
       </c>
       <c r="C573" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="574" spans="1:3" x14ac:dyDescent="0.25">
@@ -21761,7 +21761,7 @@
         <v>7</v>
       </c>
       <c r="C574" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="575" spans="1:3" x14ac:dyDescent="0.25">
@@ -21772,7 +21772,7 @@
         <v>8</v>
       </c>
       <c r="C575" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.25">
@@ -21783,7 +21783,7 @@
         <v>9</v>
       </c>
       <c r="C576" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="577" spans="1:3" x14ac:dyDescent="0.25">
@@ -21794,7 +21794,7 @@
         <v>10</v>
       </c>
       <c r="C577" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="578" spans="1:3" x14ac:dyDescent="0.25">
@@ -21805,7 +21805,7 @@
         <v>11</v>
       </c>
       <c r="C578" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="579" spans="1:3" x14ac:dyDescent="0.25">
@@ -21816,7 +21816,7 @@
         <v>12</v>
       </c>
       <c r="C579" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="580" spans="1:3" x14ac:dyDescent="0.25">
@@ -21827,7 +21827,7 @@
         <v>13</v>
       </c>
       <c r="C580" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="581" spans="1:3" x14ac:dyDescent="0.25">
@@ -21838,7 +21838,7 @@
         <v>14</v>
       </c>
       <c r="C581" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="582" spans="1:3" x14ac:dyDescent="0.25">
@@ -21849,7 +21849,7 @@
         <v>15</v>
       </c>
       <c r="C582" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="583" spans="1:3" x14ac:dyDescent="0.25">
@@ -21860,7 +21860,7 @@
         <v>16</v>
       </c>
       <c r="C583" t="s">
-        <v>3240</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="584" spans="1:3" x14ac:dyDescent="0.25">
@@ -22058,7 +22058,7 @@
         <v>4</v>
       </c>
       <c r="C601" t="s">
-        <v>3288</v>
+        <v>3287</v>
       </c>
     </row>
     <row r="602" spans="1:3" x14ac:dyDescent="0.25">
@@ -22069,7 +22069,7 @@
         <v>1</v>
       </c>
       <c r="C602" t="s">
-        <v>3241</v>
+        <v>3240</v>
       </c>
     </row>
     <row r="603" spans="1:3" x14ac:dyDescent="0.25">
@@ -22113,7 +22113,7 @@
         <v>6</v>
       </c>
       <c r="C606" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="607" spans="1:3" x14ac:dyDescent="0.25">
@@ -22124,7 +22124,7 @@
         <v>7</v>
       </c>
       <c r="C607" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="608" spans="1:3" x14ac:dyDescent="0.25">
@@ -22135,7 +22135,7 @@
         <v>8</v>
       </c>
       <c r="C608" t="s">
-        <v>3244</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="609" spans="1:3" x14ac:dyDescent="0.25">
@@ -22146,7 +22146,7 @@
         <v>9</v>
       </c>
       <c r="C609" t="s">
-        <v>3286</v>
+        <v>3285</v>
       </c>
     </row>
     <row r="610" spans="1:3" x14ac:dyDescent="0.25">
@@ -22179,7 +22179,7 @@
         <v>3</v>
       </c>
       <c r="C612" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="613" spans="1:3" x14ac:dyDescent="0.25">
@@ -22190,7 +22190,7 @@
         <v>4</v>
       </c>
       <c r="C613" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="614" spans="1:3" x14ac:dyDescent="0.25">
@@ -22201,7 +22201,7 @@
         <v>5</v>
       </c>
       <c r="C614" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="615" spans="1:3" x14ac:dyDescent="0.25">
@@ -22212,7 +22212,7 @@
         <v>6</v>
       </c>
       <c r="C615" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="616" spans="1:3" x14ac:dyDescent="0.25">
@@ -22223,7 +22223,7 @@
         <v>7</v>
       </c>
       <c r="C616" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="617" spans="1:3" x14ac:dyDescent="0.25">
@@ -22234,7 +22234,7 @@
         <v>8</v>
       </c>
       <c r="C617" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="618" spans="1:3" x14ac:dyDescent="0.25">
@@ -22245,7 +22245,7 @@
         <v>9</v>
       </c>
       <c r="C618" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="619" spans="1:3" x14ac:dyDescent="0.25">
@@ -22256,7 +22256,7 @@
         <v>10</v>
       </c>
       <c r="C619" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="620" spans="1:3" x14ac:dyDescent="0.25">
@@ -22267,7 +22267,7 @@
         <v>11</v>
       </c>
       <c r="C620" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="621" spans="1:3" x14ac:dyDescent="0.25">
@@ -22278,7 +22278,7 @@
         <v>12</v>
       </c>
       <c r="C621" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="622" spans="1:3" x14ac:dyDescent="0.25">
@@ -22289,7 +22289,7 @@
         <v>1</v>
       </c>
       <c r="C622" t="s">
-        <v>3288</v>
+        <v>3287</v>
       </c>
     </row>
     <row r="623" spans="1:3" x14ac:dyDescent="0.25">
@@ -22575,7 +22575,7 @@
         <v>3</v>
       </c>
       <c r="C648" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="649" spans="1:3" x14ac:dyDescent="0.25">
@@ -22586,7 +22586,7 @@
         <v>4</v>
       </c>
       <c r="C649" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="650" spans="1:3" x14ac:dyDescent="0.25">
@@ -22597,7 +22597,7 @@
         <v>5</v>
       </c>
       <c r="C650" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="651" spans="1:3" x14ac:dyDescent="0.25">
@@ -22608,7 +22608,7 @@
         <v>6</v>
       </c>
       <c r="C651" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="652" spans="1:3" x14ac:dyDescent="0.25">
@@ -22619,7 +22619,7 @@
         <v>7</v>
       </c>
       <c r="C652" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="653" spans="1:3" x14ac:dyDescent="0.25">
@@ -22630,7 +22630,7 @@
         <v>8</v>
       </c>
       <c r="C653" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="654" spans="1:3" x14ac:dyDescent="0.25">
@@ -22641,7 +22641,7 @@
         <v>9</v>
       </c>
       <c r="C654" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="655" spans="1:3" x14ac:dyDescent="0.25">
@@ -22652,7 +22652,7 @@
         <v>10</v>
       </c>
       <c r="C655" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="656" spans="1:3" x14ac:dyDescent="0.25">
@@ -22663,7 +22663,7 @@
         <v>11</v>
       </c>
       <c r="C656" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="657" spans="1:3" x14ac:dyDescent="0.25">
@@ -22674,7 +22674,7 @@
         <v>12</v>
       </c>
       <c r="C657" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="658" spans="1:3" x14ac:dyDescent="0.25">
@@ -22685,7 +22685,7 @@
         <v>13</v>
       </c>
       <c r="C658" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="659" spans="1:3" x14ac:dyDescent="0.25">
@@ -22696,7 +22696,7 @@
         <v>14</v>
       </c>
       <c r="C659" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="660" spans="1:3" x14ac:dyDescent="0.25">
@@ -22707,7 +22707,7 @@
         <v>15</v>
       </c>
       <c r="C660" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="661" spans="1:3" x14ac:dyDescent="0.25">
@@ -22718,7 +22718,7 @@
         <v>16</v>
       </c>
       <c r="C661" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="662" spans="1:3" x14ac:dyDescent="0.25">
@@ -22729,7 +22729,7 @@
         <v>17</v>
       </c>
       <c r="C662" t="s">
-        <v>3242</v>
+        <v>3241</v>
       </c>
     </row>
   </sheetData>
@@ -25684,19 +25684,19 @@
         <v>808</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>3227</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>3228</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="D7" s="16" t="s">
         <v>3229</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="E7" s="16" t="s">
         <v>3230</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="F7" s="16" t="s">
         <v>3231</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>3232</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>799</v>
@@ -25705,7 +25705,7 @@
         <v>821</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>3233</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -26467,10 +26467,10 @@
         <v>808</v>
       </c>
       <c r="B34" s="16" t="s">
+        <v>3219</v>
+      </c>
+      <c r="C34" s="16" t="s">
         <v>3220</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>3221</v>
       </c>
       <c r="D34" s="17">
         <v>1890</v>
@@ -26479,7 +26479,7 @@
         <v>117</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>3222</v>
+        <v>3221</v>
       </c>
       <c r="G34" s="16" t="s">
         <v>799</v>
@@ -26488,7 +26488,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>3223</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -28352,10 +28352,10 @@
         <v>808</v>
       </c>
       <c r="B99" s="16" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C99" s="16" t="s">
         <v>3234</v>
-      </c>
-      <c r="C99" s="16" t="s">
-        <v>3235</v>
       </c>
       <c r="D99" s="17">
         <v>1939</v>
@@ -28364,7 +28364,7 @@
         <v>1465</v>
       </c>
       <c r="F99" s="16" t="s">
-        <v>3236</v>
+        <v>3235</v>
       </c>
       <c r="G99" s="16" t="s">
         <v>799</v>
@@ -28373,7 +28373,7 @@
         <v>91</v>
       </c>
       <c r="I99" s="16" t="s">
-        <v>3247</v>
+        <v>3246</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -28381,19 +28381,19 @@
         <v>808</v>
       </c>
       <c r="B100" s="16" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C100" s="16" t="s">
         <v>3234</v>
-      </c>
-      <c r="C100" s="16" t="s">
-        <v>3235</v>
       </c>
       <c r="D100" s="17">
         <v>1939</v>
       </c>
       <c r="E100" s="16" t="s">
-        <v>3238</v>
+        <v>3237</v>
       </c>
       <c r="F100" s="16" t="s">
-        <v>3237</v>
+        <v>3236</v>
       </c>
       <c r="G100" s="16" t="s">
         <v>799</v>
@@ -28402,7 +28402,7 @@
         <v>39</v>
       </c>
       <c r="I100" s="16" t="s">
-        <v>3248</v>
+        <v>3247</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -28410,10 +28410,10 @@
         <v>808</v>
       </c>
       <c r="B101" s="16" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C101" s="16" t="s">
         <v>3234</v>
-      </c>
-      <c r="C101" s="16" t="s">
-        <v>3235</v>
       </c>
       <c r="D101" s="17">
         <v>1939</v>
@@ -28422,7 +28422,7 @@
         <v>108</v>
       </c>
       <c r="F101" s="16" t="s">
-        <v>3239</v>
+        <v>3238</v>
       </c>
       <c r="G101" s="16" t="s">
         <v>799</v>
@@ -28431,7 +28431,7 @@
         <v>2</v>
       </c>
       <c r="I101" s="16" t="s">
-        <v>3249</v>
+        <v>3248</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -30121,10 +30121,10 @@
         <v>808</v>
       </c>
       <c r="B160" s="16" t="s">
+        <v>3250</v>
+      </c>
+      <c r="C160" s="16" t="s">
         <v>3251</v>
-      </c>
-      <c r="C160" s="16" t="s">
-        <v>3252</v>
       </c>
       <c r="D160" s="17">
         <v>1951</v>
@@ -30133,7 +30133,7 @@
         <v>1054</v>
       </c>
       <c r="F160" s="16" t="s">
-        <v>3250</v>
+        <v>3249</v>
       </c>
       <c r="G160" s="16" t="s">
         <v>799</v>
@@ -30142,7 +30142,7 @@
         <v>78</v>
       </c>
       <c r="I160" s="16" t="s">
-        <v>3253</v>
+        <v>3252</v>
       </c>
     </row>
     <row r="161" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -43279,7 +43279,7 @@
         <v>62</v>
       </c>
       <c r="I613" s="16" t="s">
-        <v>3254</v>
+        <v>3253</v>
       </c>
     </row>
     <row r="614" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -44694,7 +44694,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -45867,7 +45867,7 @@
         <v>26</v>
       </c>
       <c r="B59" t="s">
-        <v>3285</v>
+        <v>3284</v>
       </c>
       <c r="C59" t="s">
         <v>26</v>
@@ -46201,7 +46201,7 @@
         <v>1189</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>3261</v>
+        <v>3260</v>
       </c>
       <c r="G73" s="7" t="s">
         <v>1127</v>
@@ -46902,7 +46902,7 @@
         <v>46</v>
       </c>
       <c r="B104" t="s">
-        <v>3265</v>
+        <v>3264</v>
       </c>
       <c r="C104" t="s">
         <v>46</v>
@@ -46971,7 +46971,7 @@
         <v>1099</v>
       </c>
       <c r="B107" t="s">
-        <v>3255</v>
+        <v>3254</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>91</v>
@@ -47178,7 +47178,7 @@
         <v>50</v>
       </c>
       <c r="B116" t="s">
-        <v>3258</v>
+        <v>3257</v>
       </c>
       <c r="C116" t="s">
         <v>50</v>
@@ -47914,7 +47914,7 @@
         <v>62</v>
       </c>
       <c r="B148" t="s">
-        <v>3284</v>
+        <v>3283</v>
       </c>
       <c r="C148" t="s">
         <v>62</v>
@@ -48742,7 +48742,7 @@
         <v>84</v>
       </c>
       <c r="B184" t="s">
-        <v>3257</v>
+        <v>3256</v>
       </c>
       <c r="C184" t="s">
         <v>84</v>
@@ -49222,7 +49222,7 @@
         <v>2906</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>3266</v>
+        <v>3265</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>2907</v>
@@ -49701,7 +49701,7 @@
         <v>2931</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>3267</v>
+        <v>3266</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -49837,7 +49837,7 @@
         <v>2950</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>3267</v>
+        <v>3266</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -50019,11 +50019,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="19" max="19" width="8.75" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -50086,7 +50089,7 @@
         <v>3104</v>
       </c>
       <c r="B8" t="s">
-        <v>3224</v>
+        <v>3223</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -50094,7 +50097,7 @@
         <v>3106</v>
       </c>
       <c r="B9" t="s">
-        <v>3226</v>
+        <v>3225</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -50102,7 +50105,7 @@
         <v>3104</v>
       </c>
       <c r="B10" t="s">
-        <v>3225</v>
+        <v>3224</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -50110,7 +50113,7 @@
         <v>3106</v>
       </c>
       <c r="B11" t="s">
-        <v>3227</v>
+        <v>3226</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -50310,7 +50313,7 @@
         <v>3104</v>
       </c>
       <c r="B37" t="s">
-        <v>3219</v>
+        <v>3293</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -50558,7 +50561,7 @@
         <v>3102</v>
       </c>
       <c r="B74" t="s">
-        <v>3259</v>
+        <v>3258</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -50566,7 +50569,7 @@
         <v>3104</v>
       </c>
       <c r="B75" t="s">
-        <v>3262</v>
+        <v>3261</v>
       </c>
     </row>
   </sheetData>
@@ -50591,18 +50594,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>3270</v>
+        <v>3269</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>3268</v>
+        <v>3267</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>821</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>3269</v>
+        <v>3268</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -50679,7 +50682,7 @@
         <v>1127</v>
       </c>
       <c r="C9" t="s">
-        <v>3279</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -50690,7 +50693,7 @@
         <v>1127</v>
       </c>
       <c r="C10" t="s">
-        <v>3280</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -50734,7 +50737,7 @@
         <v>1127</v>
       </c>
       <c r="C14" t="s">
-        <v>3281</v>
+        <v>3280</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -50750,18 +50753,18 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>3271</v>
+        <v>3270</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
+        <v>3271</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>3272</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>3273</v>
-      </c>
       <c r="C19" s="22" t="s">
-        <v>3269</v>
+        <v>3268</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -50794,7 +50797,7 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -50802,10 +50805,10 @@
         <v>2018</v>
       </c>
       <c r="B23" t="s">
-        <v>3277</v>
+        <v>3276</v>
       </c>
       <c r="C23" t="s">
-        <v>3282</v>
+        <v>3281</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -50832,40 +50835,40 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>3274</v>
+        <v>3273</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>3283</v>
+        <v>3282</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>3273</v>
+        <v>3272</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>3269</v>
+        <v>3268</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>3275</v>
+        <v>3274</v>
       </c>
       <c r="B30" t="s">
         <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>3276</v>
+        <v>3275</v>
       </c>
       <c r="B31" t="s">
         <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>3278</v>
+        <v>3277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added misspelling of seismella
</commit_message>
<xml_diff>
--- a/data/Species DB.xlsx
+++ b/data/Species DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8130" yWindow="525" windowWidth="10500" windowHeight="13155" activeTab="7"/>
+    <workbookView xWindow="8130" yWindow="525" windowWidth="10500" windowHeight="13155" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="species_info" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10421" uniqueCount="3294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10421" uniqueCount="3295">
   <si>
     <t>acuta</t>
   </si>
@@ -9904,6 +9904,9 @@
   </si>
   <si>
     <t>Less commonly used in English, the term &amp;ldquo;Calling Crab&amp;rdquo; derives from one of the earliest scientific papers to include these crabs, [[Rumphius1705,.out]]. Rumphius names one of his species &lt;em class="species"&gt;Cancer vocans&lt;/em&gt;  which is Latin for &amp;ldquo;calling crab&amp;rdquo; or &amp;ldquo;gesturing crab.&amp;rdquo; He also reports the name &amp;ldquo;Cattam Pangel&amp;rdquo; which appears to most likely be a form of Malay meaning &amp;ldquo;summoning crab,&amp;rdquo; and is probably from where he derived the Latin name. In a later work ([[Rumphius1711,.in]]) he includes a Dutch name &amp;ldquo;Roepende Krabbe,&amp;rdquo; which also translates to Calling Crab.</t>
+  </si>
+  <si>
+    <t>seismella;siesmella</t>
   </si>
 </sst>
 </file>
@@ -44513,8 +44516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A161" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48259,7 +48262,7 @@
         <v>69</v>
       </c>
       <c r="B163" t="s">
-        <v>69</v>
+        <v>3294</v>
       </c>
       <c r="C163" t="s">
         <v>69</v>
@@ -50019,7 +50022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
major location hierarchy update
</commit_message>
<xml_diff>
--- a/data/Species DB.xlsx
+++ b/data/Species DB.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox (Personal)\Webpages\TaxonomyMonographBuilder\fiddlercrab.info\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8130" yWindow="525" windowWidth="10500" windowHeight="13155" activeTab="4"/>
+    <workbookView xWindow="8130" yWindow="525" windowWidth="10500" windowHeight="13155" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species_info" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10429" uniqueCount="3304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10429" uniqueCount="3305">
   <si>
     <t>acuta</t>
   </si>
@@ -9934,12 +9939,15 @@
   </si>
   <si>
     <t>This drawing is from Pesta (1911). He labeled it &lt;em class="species"&gt;Uca gaimardi.&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>festae;festæ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -10119,7 +10127,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10152,9 +10160,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10187,6 +10212,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -10362,7 +10404,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10372,13 +10414,13 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="4" max="4" width="17.375" customWidth="1"/>
-    <col min="5" max="5" width="21.25" customWidth="1"/>
-    <col min="6" max="6" width="9.625" customWidth="1"/>
-    <col min="7" max="7" width="19.125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
     <col min="8" max="8" width="77" customWidth="1"/>
-    <col min="9" max="9" width="17.125" customWidth="1"/>
-    <col min="11" max="11" width="12.625" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
@@ -15187,7 +15229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15196,9 +15238,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.75" customWidth="1"/>
-    <col min="2" max="2" width="27.375" customWidth="1"/>
-    <col min="3" max="3" width="9.375" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -15468,7 +15510,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C662"/>
   <sheetViews>
     <sheetView topLeftCell="A598" workbookViewId="0">
@@ -15477,7 +15519,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.625" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -22773,7 +22815,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22783,9 +22825,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="4.75" customWidth="1"/>
-    <col min="4" max="4" width="13.75" customWidth="1"/>
-    <col min="8" max="8" width="43.75" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
@@ -25515,24 +25557,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="15"/>
-    <col min="3" max="3" width="18.375" style="15" customWidth="1"/>
-    <col min="4" max="4" width="6.75" style="15" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="15"/>
+    <col min="3" max="3" width="18.42578125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="15" customWidth="1"/>
     <col min="5" max="6" width="21" style="15" customWidth="1"/>
-    <col min="7" max="7" width="6.75" style="15" customWidth="1"/>
-    <col min="8" max="8" width="9.375" style="15" customWidth="1"/>
-    <col min="9" max="16" width="9.125" style="15"/>
-    <col min="17" max="17" width="9.625" style="15" customWidth="1"/>
-    <col min="18" max="16384" width="9.125" style="15"/>
+    <col min="7" max="7" width="6.7109375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="15" customWidth="1"/>
+    <col min="9" max="16" width="9.140625" style="15"/>
+    <col min="17" max="17" width="9.5703125" style="15" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -44569,22 +44611,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
-    <col min="2" max="2" width="38.625" customWidth="1"/>
-    <col min="3" max="3" width="9.75" customWidth="1"/>
-    <col min="4" max="4" width="17.375" customWidth="1"/>
-    <col min="5" max="5" width="18.875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="21.875" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -45903,7 +45945,7 @@
         <v>25</v>
       </c>
       <c r="B58" t="s">
-        <v>25</v>
+        <v>3304</v>
       </c>
       <c r="C58" t="s">
         <v>25</v>
@@ -49220,7 +49262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -49229,11 +49271,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.625" customWidth="1"/>
-    <col min="2" max="2" width="13.875" customWidth="1"/>
-    <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="22.75" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -50075,7 +50117,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -50084,7 +50126,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="8.75" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -50638,7 +50680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -50647,7 +50689,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.375" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
added missing species update
forgot to put occidentalis on the new species table
</commit_message>
<xml_diff>
--- a/data/Species DB.xlsx
+++ b/data/Species DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox (Personal)\Webpages\TaxonomyMonographBuilder\fiddlercrab.info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C0364C-4C28-415A-BA82-4BD285F877D1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FE7A61-4603-4580-A253-80B77369BD72}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8130" yWindow="525" windowWidth="10500" windowHeight="13155" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8130" yWindow="525" windowWidth="10500" windowHeight="13155" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species_info" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10485" uniqueCount="3328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10488" uniqueCount="3328">
   <si>
     <t>acuta</t>
   </si>
@@ -44902,7 +44902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
@@ -50969,10 +50969,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51140,39 +51140,39 @@
         <v>2857</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>3253</v>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3126</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3128</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
+        <v>3253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
         <v>3254</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B20" s="22" t="s">
         <v>3255</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C20" s="22" t="s">
         <v>3251</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>2015</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>2518</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>2152</v>
+        <v>2015</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
         <v>2518</v>
@@ -51180,83 +51180,94 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>2519</v>
+        <v>2152</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>3260</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2011</v>
+        <v>2519</v>
       </c>
       <c r="B23" t="s">
-        <v>3259</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>3264</v>
+        <v>3260</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2161</v>
+        <v>2011</v>
       </c>
       <c r="B24" t="s">
-        <v>1081</v>
+        <v>3259</v>
       </c>
       <c r="C24" t="s">
-        <v>1122</v>
+        <v>3264</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>2161</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>1313</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>25</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>3193</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
-        <v>3256</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
+        <v>3256</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
         <v>3265</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B30" s="22" t="s">
         <v>3255</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C30" s="22" t="s">
         <v>3251</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>3257</v>
-      </c>
-      <c r="B30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" t="s">
-        <v>3260</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>3257</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>3258</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>49</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>3260</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removing ae and oe ligatures as separate spellings
</commit_message>
<xml_diff>
--- a/data/Species DB.xlsx
+++ b/data/Species DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Webpages\TaxonomyMonographBuilder\fiddlercrab.info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6797A4-C571-4E5B-AB3D-99C251DDAE1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84485BD4-B0B3-4426-808A-869EC7EC5B18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3456" yWindow="108" windowWidth="18240" windowHeight="16572" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="84" yWindow="24" windowWidth="18240" windowHeight="16572" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species" sheetId="1" r:id="rId1"/>
@@ -17178,7 +17178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7951029-2498-4E57-BAA0-E3E88F91FE9E}">
   <dimension ref="A1:E776"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A472" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B483" sqref="B483"/>
     </sheetView>
@@ -60532,8 +60532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G202"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>